<commit_message>
dev excel user report
</commit_message>
<xml_diff>
--- a/resources/templete/report.xlsx
+++ b/resources/templete/report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Task Report</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,27 +55,48 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>장비 접속여부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">등록 유저 수 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>에러 로그</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>220.64.140.216</t>
+  </si>
+  <si>
+    <t>SE-IBP-DEVELOP-3560-03</t>
+  </si>
+  <si>
     <t>성공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에러</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>220.64.140.217</t>
+  </si>
+  <si>
+    <t>SE-IBP-DEVELOP-3560-02</t>
+  </si>
+  <si>
+    <t>220.64.140.218</t>
+  </si>
+  <si>
+    <t>SE-IBP-DEVELOP-3560-01</t>
+  </si>
+  <si>
+    <t>220.64.140.219</t>
   </si>
   <si>
     <t>실패</t>
+  </si>
+  <si>
+    <t>[LOGINFAIL] 220.64.140.219 : java.net.ConnectException: Connection refused: connect</t>
+  </si>
+  <si>
+    <t>접속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">유저 수 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -83,6 +104,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -241,7 +265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -254,20 +278,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -592,52 +622,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.25" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.75" style="4" customWidth="1"/>
     <col min="6" max="16384" width="16.25" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="16.5">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="12"/>
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
-        <v>41760.347222222219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:5" ht="16.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="10">
+        <v>41760.347222222219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -645,7 +675,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -655,55 +685,97 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="3">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="36">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>13</v>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +786,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"실패"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>